<commit_message>
presentation full and metrics
</commit_message>
<xml_diff>
--- a/metrics/metrics.xlsx
+++ b/metrics/metrics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="metrics" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="14">
   <si>
     <t xml:space="preserve">DATASETS</t>
   </si>
@@ -239,18 +239,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:AD59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T44" activeCellId="0" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,6 +315,33 @@
         <v>10</v>
       </c>
       <c r="U1" s="1"/>
+      <c r="V1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -389,6 +416,33 @@
         <f aca="false">S2/1000</f>
         <v>5.2434</v>
       </c>
+      <c r="V2" s="0" t="n">
+        <v>7058</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>6702</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <v>6807</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <v>6805</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>6765</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <f aca="false">MIN(V2:Z2)</f>
+        <v>6702</v>
+      </c>
+      <c r="AC2" s="0" t="n">
+        <f aca="false">AVERAGE(V2:Z2)</f>
+        <v>6827.4</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <f aca="false">AC2/1000</f>
+        <v>6.8274</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -463,6 +517,33 @@
         <f aca="false">S3/1000</f>
         <v>4.5594</v>
       </c>
+      <c r="V3" s="0" t="n">
+        <v>8031</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>7849</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>8125</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>7866</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>7645</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <f aca="false">MIN(V3:Z3)</f>
+        <v>7645</v>
+      </c>
+      <c r="AC3" s="0" t="n">
+        <f aca="false">AVERAGE(V3:Z3)</f>
+        <v>7903.2</v>
+      </c>
+      <c r="AD3" s="0" t="n">
+        <f aca="false">AC3/1000</f>
+        <v>7.9032</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -537,6 +618,33 @@
         <f aca="false">S4/1000</f>
         <v>4.025</v>
       </c>
+      <c r="V4" s="0" t="n">
+        <v>9548</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>9580</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>9648</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>9490</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>9194</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <f aca="false">MIN(V4:Z4)</f>
+        <v>9194</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <f aca="false">AVERAGE(V4:Z4)</f>
+        <v>9492</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <f aca="false">AC4/1000</f>
+        <v>9.492</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -611,6 +719,33 @@
         <f aca="false">S5/1000</f>
         <v>4.237</v>
       </c>
+      <c r="V5" s="0" t="n">
+        <v>13328</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>13318</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>13344</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>13633</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>13950</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <f aca="false">MIN(V5:Z5)</f>
+        <v>13318</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <f aca="false">AVERAGE(V5:Z5)</f>
+        <v>13514.6</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <f aca="false">AC5/1000</f>
+        <v>13.5146</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -650,25 +785,67 @@
         <f aca="false">J$2/J6</f>
         <v>5.72435767459375</v>
       </c>
+      <c r="L6" s="0" t="n">
+        <v>5459</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>5275</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>5190</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>5265</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>4863</v>
+      </c>
       <c r="Q6" s="0" t="n">
         <f aca="false">MIN(L6:P6)</f>
-        <v>0</v>
+        <v>4863</v>
       </c>
       <c r="R6" s="0" t="n">
         <f aca="false">MAX(L6:P6)</f>
-        <v>0</v>
-      </c>
-      <c r="S6" s="0" t="e">
+        <v>5459</v>
+      </c>
+      <c r="S6" s="0" t="n">
         <f aca="false">AVERAGE(L6:P6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T6" s="0" t="e">
+        <v>5210.4</v>
+      </c>
+      <c r="T6" s="0" t="n">
         <f aca="false">S$2/S6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U6" s="0" t="e">
+        <v>1.00633348687241</v>
+      </c>
+      <c r="U6" s="0" t="n">
         <f aca="false">S6/1000</f>
-        <v>#DIV/0!</v>
+        <v>5.2104</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>18615</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>17990</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>18530</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>19163</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>18698</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <f aca="false">MIN(V6:Z6)</f>
+        <v>17990</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <f aca="false">AVERAGE(V6:Z6)</f>
+        <v>18599.2</v>
+      </c>
+      <c r="AD6" s="0" t="n">
+        <f aca="false">AC6/1000</f>
+        <v>18.5992</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,6 +921,18 @@
         <f aca="false">S7/1000</f>
         <v>6.8274</v>
       </c>
+      <c r="AA7" s="0" t="n">
+        <f aca="false">MIN(V7:Z7)</f>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="0" t="e">
+        <f aca="false">AVERAGE(V7:Z7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD7" s="0" t="e">
+        <f aca="false">AC7/1000</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -818,6 +1007,33 @@
         <f aca="false">S8/1000</f>
         <v>21.1148</v>
       </c>
+      <c r="V8" s="0" t="n">
+        <v>8959</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>9373</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <v>9108</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <v>9015</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <v>9527</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <f aca="false">MIN(V8:Z8)</f>
+        <v>8959</v>
+      </c>
+      <c r="AC8" s="0" t="n">
+        <f aca="false">AVERAGE(V8:Z8)</f>
+        <v>9196.4</v>
+      </c>
+      <c r="AD8" s="0" t="n">
+        <f aca="false">AC8/1000</f>
+        <v>9.1964</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -892,6 +1108,33 @@
         <f aca="false">S9/1000</f>
         <v>14.9388</v>
       </c>
+      <c r="V9" s="0" t="n">
+        <v>10300</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>9619</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>10046</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>9980</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>9655</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <f aca="false">MIN(V9:Z9)</f>
+        <v>9619</v>
+      </c>
+      <c r="AC9" s="0" t="n">
+        <f aca="false">AVERAGE(V9:Z9)</f>
+        <v>9920</v>
+      </c>
+      <c r="AD9" s="0" t="n">
+        <f aca="false">AC9/1000</f>
+        <v>9.92</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -966,6 +1209,33 @@
         <f aca="false">S10/1000</f>
         <v>10.1884</v>
       </c>
+      <c r="V10" s="0" t="n">
+        <v>12411</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>12644</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <v>12200</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>12212</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>12192</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <f aca="false">MIN(V10:Z10)</f>
+        <v>12192</v>
+      </c>
+      <c r="AC10" s="0" t="n">
+        <f aca="false">AVERAGE(V10:Z10)</f>
+        <v>12331.8</v>
+      </c>
+      <c r="AD10" s="0" t="n">
+        <f aca="false">AC10/1000</f>
+        <v>12.3318</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -1040,6 +1310,33 @@
         <f aca="false">S11/1000</f>
         <v>8.1612</v>
       </c>
+      <c r="V11" s="0" t="n">
+        <v>15827</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>15724</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <v>15917</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <v>16046</v>
+      </c>
+      <c r="Z11" s="0" t="n">
+        <v>15508</v>
+      </c>
+      <c r="AA11" s="0" t="n">
+        <f aca="false">MIN(V11:Z11)</f>
+        <v>15508</v>
+      </c>
+      <c r="AC11" s="0" t="n">
+        <f aca="false">AVERAGE(V11:Z11)</f>
+        <v>15804.4</v>
+      </c>
+      <c r="AD11" s="0" t="n">
+        <f aca="false">AC11/1000</f>
+        <v>15.8044</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -1079,25 +1376,67 @@
         <f aca="false">J$8/J12</f>
         <v>6.66926174424625</v>
       </c>
+      <c r="L12" s="0" t="n">
+        <v>7342</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>7496</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>7201</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>7063</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>7387</v>
+      </c>
       <c r="Q12" s="0" t="n">
         <f aca="false">MIN(L12:P12)</f>
-        <v>0</v>
+        <v>7063</v>
       </c>
       <c r="R12" s="0" t="n">
         <f aca="false">MAX(L12:P12)</f>
-        <v>0</v>
-      </c>
-      <c r="S12" s="0" t="e">
+        <v>7496</v>
+      </c>
+      <c r="S12" s="0" t="n">
         <f aca="false">AVERAGE(L12:P12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T12" s="0" t="e">
+        <v>7297.8</v>
+      </c>
+      <c r="T12" s="0" t="n">
         <f aca="false">S$8/S12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U12" s="0" t="e">
+        <v>2.89331031269698</v>
+      </c>
+      <c r="U12" s="0" t="n">
         <f aca="false">S12/1000</f>
-        <v>#DIV/0!</v>
+        <v>7.2978</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>21802</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>22411</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <v>21831</v>
+      </c>
+      <c r="Y12" s="0" t="n">
+        <v>21990</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <v>22584</v>
+      </c>
+      <c r="AA12" s="0" t="n">
+        <f aca="false">MIN(V12:Z12)</f>
+        <v>21802</v>
+      </c>
+      <c r="AC12" s="0" t="n">
+        <f aca="false">AVERAGE(V12:Z12)</f>
+        <v>22123.6</v>
+      </c>
+      <c r="AD12" s="0" t="n">
+        <f aca="false">AC12/1000</f>
+        <v>22.1236</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,6 +1512,18 @@
         <f aca="false">S13/1000</f>
         <v>9.1964</v>
       </c>
+      <c r="AA13" s="0" t="n">
+        <f aca="false">MIN(V13:Z13)</f>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="0" t="e">
+        <f aca="false">AVERAGE(V13:Z13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD13" s="0" t="e">
+        <f aca="false">AC13/1000</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -1247,6 +1598,33 @@
         <f aca="false">S14/1000</f>
         <v>42.796</v>
       </c>
+      <c r="V14" s="0" t="n">
+        <v>13563</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>13621</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>13266</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>13791</v>
+      </c>
+      <c r="Z14" s="0" t="n">
+        <v>13371</v>
+      </c>
+      <c r="AA14" s="0" t="n">
+        <f aca="false">MIN(V14:Z14)</f>
+        <v>13266</v>
+      </c>
+      <c r="AC14" s="0" t="n">
+        <f aca="false">AVERAGE(V14:Z14)</f>
+        <v>13522.4</v>
+      </c>
+      <c r="AD14" s="0" t="n">
+        <f aca="false">AC14/1000</f>
+        <v>13.5224</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -1321,6 +1699,33 @@
         <f aca="false">S15/1000</f>
         <v>28.1094</v>
       </c>
+      <c r="V15" s="0" t="n">
+        <v>14756</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>14994</v>
+      </c>
+      <c r="X15" s="0" t="n">
+        <v>15005</v>
+      </c>
+      <c r="Y15" s="0" t="n">
+        <v>14881</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <v>15422</v>
+      </c>
+      <c r="AA15" s="0" t="n">
+        <f aca="false">MIN(V15:Z15)</f>
+        <v>14756</v>
+      </c>
+      <c r="AC15" s="0" t="n">
+        <f aca="false">AVERAGE(V15:Z15)</f>
+        <v>15011.6</v>
+      </c>
+      <c r="AD15" s="0" t="n">
+        <f aca="false">AC15/1000</f>
+        <v>15.0116</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -1395,6 +1800,33 @@
         <f aca="false">S16/1000</f>
         <v>18.4616</v>
       </c>
+      <c r="V16" s="0" t="n">
+        <v>16611</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>18181</v>
+      </c>
+      <c r="X16" s="0" t="n">
+        <v>16527</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <v>17538</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <v>17042</v>
+      </c>
+      <c r="AA16" s="0" t="n">
+        <f aca="false">MIN(V16:Z16)</f>
+        <v>16527</v>
+      </c>
+      <c r="AC16" s="0" t="n">
+        <f aca="false">AVERAGE(V16:Z16)</f>
+        <v>17179.8</v>
+      </c>
+      <c r="AD16" s="0" t="n">
+        <f aca="false">AC16/1000</f>
+        <v>17.1798</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -1469,6 +1901,33 @@
         <f aca="false">S17/1000</f>
         <v>14.3632</v>
       </c>
+      <c r="V17" s="0" t="n">
+        <v>21379</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>21481</v>
+      </c>
+      <c r="X17" s="0" t="n">
+        <v>22110</v>
+      </c>
+      <c r="Y17" s="0" t="n">
+        <v>21373</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <v>21639</v>
+      </c>
+      <c r="AA17" s="0" t="n">
+        <f aca="false">MIN(V17:Z17)</f>
+        <v>21373</v>
+      </c>
+      <c r="AC17" s="0" t="n">
+        <f aca="false">AVERAGE(V17:Z17)</f>
+        <v>21596.4</v>
+      </c>
+      <c r="AD17" s="0" t="n">
+        <f aca="false">AC17/1000</f>
+        <v>21.5964</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -1508,25 +1967,67 @@
         <f aca="false">J$14/J18</f>
         <v>7.72118886811282</v>
       </c>
+      <c r="L18" s="0" t="n">
+        <v>12295</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>12039</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>12310</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>11722</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>12172</v>
+      </c>
       <c r="Q18" s="0" t="n">
         <f aca="false">MIN(L18:P18)</f>
-        <v>0</v>
+        <v>11722</v>
       </c>
       <c r="R18" s="0" t="n">
         <f aca="false">MAX(L18:P18)</f>
-        <v>0</v>
-      </c>
-      <c r="S18" s="0" t="e">
+        <v>12310</v>
+      </c>
+      <c r="S18" s="0" t="n">
         <f aca="false">AVERAGE(L18:P18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T18" s="0" t="e">
+        <v>12107.6</v>
+      </c>
+      <c r="T18" s="0" t="n">
         <f aca="false">S$14/S18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U18" s="0" t="e">
+        <v>3.53463940004625</v>
+      </c>
+      <c r="U18" s="0" t="n">
         <f aca="false">S18/1000</f>
-        <v>#DIV/0!</v>
+        <v>12.1076</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <v>28438</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>27787</v>
+      </c>
+      <c r="X18" s="0" t="n">
+        <v>28270</v>
+      </c>
+      <c r="Y18" s="0" t="n">
+        <v>28180</v>
+      </c>
+      <c r="Z18" s="0" t="n">
+        <v>28973</v>
+      </c>
+      <c r="AA18" s="0" t="n">
+        <f aca="false">MIN(V18:Z18)</f>
+        <v>27787</v>
+      </c>
+      <c r="AC18" s="0" t="n">
+        <f aca="false">AVERAGE(V18:Z18)</f>
+        <v>28329.6</v>
+      </c>
+      <c r="AD18" s="0" t="n">
+        <f aca="false">AC18/1000</f>
+        <v>28.3296</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,34 +2103,46 @@
         <f aca="false">S19/1000</f>
         <v>13.5224</v>
       </c>
+      <c r="AA19" s="0" t="n">
+        <f aca="false">MIN(V19:Z19)</f>
+        <v>0</v>
+      </c>
+      <c r="AC19" s="0" t="e">
+        <f aca="false">AVERAGE(V19:Z19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD19" s="0" t="e">
+        <f aca="false">AC19/1000</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="n">
-        <v>0.293007</v>
+        <v>0.29342</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>0.207788</v>
+        <v>0.288763</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>0.259716</v>
+        <v>0.285342</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>0.276858</v>
+        <v>0.296652</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>0.288596</v>
+        <v>0.290754</v>
       </c>
       <c r="H22" s="0" t="n">
         <f aca="false">MIN(C22:G22)</f>
-        <v>0.207788</v>
+        <v>0.285342</v>
       </c>
       <c r="I22" s="0" t="n">
         <f aca="false">MAX(C22:G22)</f>
-        <v>0.293007</v>
+        <v>0.296652</v>
       </c>
       <c r="J22" s="0" t="n">
         <f aca="false">AVERAGE(C22:G22)</f>
-        <v>0.265193</v>
+        <v>0.2909862</v>
       </c>
       <c r="K22" s="0" t="n">
         <f aca="false">J$22/J22</f>
@@ -1638,196 +2151,196 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="n">
-        <v>0.150373</v>
+        <v>0.150208</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>0.154229</v>
+        <v>0.162441</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>0.154739</v>
+        <v>0.154983</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>0.165948</v>
+        <v>0.166783</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>0.163992</v>
+        <v>0.161101</v>
       </c>
       <c r="H23" s="0" t="n">
         <f aca="false">MIN(C23:G23)</f>
-        <v>0.150373</v>
+        <v>0.150208</v>
       </c>
       <c r="I23" s="0" t="n">
         <f aca="false">MAX(C23:G23)</f>
-        <v>0.165948</v>
+        <v>0.166783</v>
       </c>
       <c r="J23" s="0" t="n">
         <f aca="false">AVERAGE(C23:G23)</f>
-        <v>0.1578562</v>
+        <v>0.1591032</v>
       </c>
       <c r="K23" s="0" t="n">
         <f aca="false">J$22/J23</f>
-        <v>1.67996569029281</v>
+        <v>1.82891481755238</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="n">
-        <v>0.096497</v>
+        <v>0.094023</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>0.092027</v>
+        <v>0.091874</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>0.091783</v>
+        <v>0.093575</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>0.091716</v>
+        <v>0.095933</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>0.095108</v>
+        <v>0.095697</v>
       </c>
       <c r="H24" s="0" t="n">
         <f aca="false">MIN(C24:G24)</f>
-        <v>0.091716</v>
+        <v>0.091874</v>
       </c>
       <c r="I24" s="0" t="n">
         <f aca="false">MAX(C24:G24)</f>
-        <v>0.096497</v>
+        <v>0.095933</v>
       </c>
       <c r="J24" s="0" t="n">
         <f aca="false">AVERAGE(C24:G24)</f>
-        <v>0.0934262</v>
+        <v>0.0942204</v>
       </c>
       <c r="K24" s="0" t="n">
         <f aca="false">J$22/J24</f>
-        <v>2.83852923483991</v>
+        <v>3.08835666161468</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="n">
-        <v>0.054706</v>
+        <v>0.054374</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>0.054979</v>
+        <v>0.072948</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>0.055075</v>
+        <v>0.054812</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>0.054461</v>
+        <v>0.056093</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>0.07164</v>
+        <v>0.053685</v>
       </c>
       <c r="H25" s="0" t="n">
         <f aca="false">MIN(C25:G25)</f>
-        <v>0.054461</v>
+        <v>0.053685</v>
       </c>
       <c r="I25" s="0" t="n">
         <f aca="false">MAX(C25:G25)</f>
-        <v>0.07164</v>
+        <v>0.072948</v>
       </c>
       <c r="J25" s="0" t="n">
         <f aca="false">AVERAGE(C25:G25)</f>
-        <v>0.0581722</v>
+        <v>0.0583824</v>
       </c>
       <c r="K25" s="0" t="n">
         <f aca="false">J$22/J25</f>
-        <v>4.55875830723266</v>
+        <v>4.98414248129573</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="n">
-        <v>0.052315</v>
+        <v>0.053995</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0.052957</v>
+        <v>0.07</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>0.052421</v>
+        <v>0.052986</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>0.052379</v>
+        <v>0.051697</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0.05032</v>
+        <v>0.054528</v>
       </c>
       <c r="H26" s="0" t="n">
         <f aca="false">MIN(C26:G26)</f>
-        <v>0.05032</v>
+        <v>0.051697</v>
       </c>
       <c r="I26" s="0" t="n">
         <f aca="false">MAX(C26:G26)</f>
-        <v>0.052957</v>
+        <v>0.07</v>
       </c>
       <c r="J26" s="0" t="n">
         <f aca="false">AVERAGE(C26:G26)</f>
-        <v>0.0520784</v>
+        <v>0.0566412</v>
       </c>
       <c r="K26" s="0" t="n">
         <f aca="false">J$22/J26</f>
-        <v>5.09218793204092</v>
+        <v>5.13735937797928</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="n">
-        <v>0.042687</v>
+        <v>0.042807</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0.03722</v>
+        <v>0.037652</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>0.042387</v>
+        <v>0.041446</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>0.044231</v>
+        <v>0.040234</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>0.040916</v>
+        <v>0.043222</v>
       </c>
       <c r="H27" s="0" t="n">
         <f aca="false">MIN(C27:G27)</f>
-        <v>0.03722</v>
+        <v>0.037652</v>
       </c>
       <c r="I27" s="0" t="n">
         <f aca="false">MAX(C27:G27)</f>
-        <v>0.044231</v>
+        <v>0.043222</v>
       </c>
       <c r="J27" s="0" t="n">
         <f aca="false">AVERAGE(C27:G27)</f>
-        <v>0.0414882</v>
+        <v>0.0410722</v>
       </c>
       <c r="K27" s="0" t="n">
         <f aca="false">J$22/J27</f>
-        <v>6.39201025833851</v>
+        <v>7.08474832124892</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="n">
-        <v>2.188911</v>
+        <v>2.130716</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>2.008085</v>
+        <v>1.966764</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>1.987982</v>
+        <v>2.143703</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>2.318396</v>
+        <v>1.919574</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>1.993888</v>
+        <v>1.992869</v>
       </c>
       <c r="H28" s="0" t="n">
         <f aca="false">MIN(C28:G28)</f>
-        <v>1.987982</v>
+        <v>1.919574</v>
       </c>
       <c r="I28" s="0" t="n">
         <f aca="false">MAX(C28:G28)</f>
-        <v>2.318396</v>
+        <v>2.143703</v>
       </c>
       <c r="J28" s="0" t="n">
         <f aca="false">AVERAGE(C28:G28)</f>
-        <v>2.0994524</v>
+        <v>2.0307252</v>
       </c>
       <c r="K28" s="0" t="n">
         <f aca="false">J$28/J28</f>
@@ -1836,196 +2349,196 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="n">
-        <v>1.190473</v>
+        <v>1.182835</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>1.261723</v>
+        <v>1.121425</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>1.286573</v>
+        <v>1.140883</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>1.301045</v>
+        <v>1.107231</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>1.29403</v>
+        <v>1.117318</v>
       </c>
       <c r="H29" s="0" t="n">
         <f aca="false">MIN(C29:G29)</f>
-        <v>1.190473</v>
+        <v>1.107231</v>
       </c>
       <c r="I29" s="0" t="n">
         <f aca="false">MAX(C29:G29)</f>
-        <v>1.301045</v>
+        <v>1.182835</v>
       </c>
       <c r="J29" s="0" t="n">
         <f aca="false">AVERAGE(C29:G29)</f>
-        <v>1.2667688</v>
+        <v>1.1339384</v>
       </c>
       <c r="K29" s="0" t="n">
         <f aca="false">J$28/J29</f>
-        <v>1.65732878801562</v>
+        <v>1.79086024426018</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="n">
-        <v>0.626066</v>
+        <v>0.664014</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0.710086</v>
+        <v>0.67292</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>0.655001</v>
+        <v>0.665489</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>0.704695</v>
+        <v>0.70704</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>0.712209</v>
+        <v>0.613855</v>
       </c>
       <c r="H30" s="0" t="n">
         <f aca="false">MIN(C30:G30)</f>
-        <v>0.626066</v>
+        <v>0.613855</v>
       </c>
       <c r="I30" s="0" t="n">
         <f aca="false">MAX(C30:G30)</f>
-        <v>0.712209</v>
+        <v>0.70704</v>
       </c>
       <c r="J30" s="0" t="n">
         <f aca="false">AVERAGE(C30:G30)</f>
-        <v>0.6816114</v>
+        <v>0.6646636</v>
       </c>
       <c r="K30" s="0" t="n">
         <f aca="false">J$28/J30</f>
-        <v>3.08013099546164</v>
+        <v>3.05526765720283</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="n">
-        <v>0.345667</v>
+        <v>0.348636</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0.389951</v>
+        <v>0.383102</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>0.357631</v>
+        <v>0.344335</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>0.358902</v>
+        <v>0.392488</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>0.381989</v>
+        <v>0.360729</v>
       </c>
       <c r="H31" s="0" t="n">
         <f aca="false">MIN(C31:G31)</f>
-        <v>0.345667</v>
+        <v>0.344335</v>
       </c>
       <c r="I31" s="0" t="n">
         <f aca="false">MAX(C31:G31)</f>
-        <v>0.389951</v>
+        <v>0.392488</v>
       </c>
       <c r="J31" s="0" t="n">
         <f aca="false">AVERAGE(C31:G31)</f>
-        <v>0.366828</v>
+        <v>0.365858</v>
       </c>
       <c r="K31" s="0" t="n">
         <f aca="false">J$28/J31</f>
-        <v>5.72326103787061</v>
+        <v>5.55058301308158</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="n">
-        <v>0.289399</v>
+        <v>0.295592</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>0.30294</v>
+        <v>0.312317</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>0.288363</v>
+        <v>0.308078</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>0.325529</v>
+        <v>0.316504</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>0.290939</v>
+        <v>0.3061</v>
       </c>
       <c r="H32" s="0" t="n">
         <f aca="false">MIN(C32:G32)</f>
-        <v>0.288363</v>
+        <v>0.295592</v>
       </c>
       <c r="I32" s="0" t="n">
         <f aca="false">MAX(C32:G32)</f>
-        <v>0.325529</v>
+        <v>0.316504</v>
       </c>
       <c r="J32" s="0" t="n">
         <f aca="false">AVERAGE(C32:G32)</f>
-        <v>0.299434</v>
+        <v>0.3077182</v>
       </c>
       <c r="K32" s="0" t="n">
         <f aca="false">J$28/J32</f>
-        <v>7.01140284670411</v>
+        <v>6.59930156877299</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="n">
-        <v>0.174582</v>
+        <v>0.196993</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>0.191944</v>
+        <v>0.190734</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>0.174624</v>
+        <v>0.189884</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>0.190995</v>
+        <v>0.177453</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>0.185192</v>
+        <v>0.187844</v>
       </c>
       <c r="H33" s="0" t="n">
         <f aca="false">MIN(C33:G33)</f>
-        <v>0.174582</v>
+        <v>0.177453</v>
       </c>
       <c r="I33" s="0" t="n">
         <f aca="false">MAX(C33:G33)</f>
-        <v>0.191944</v>
+        <v>0.196993</v>
       </c>
       <c r="J33" s="0" t="n">
         <f aca="false">AVERAGE(C33:G33)</f>
-        <v>0.1834674</v>
+        <v>0.1885816</v>
       </c>
       <c r="K33" s="0" t="n">
         <f aca="false">J$28/J33</f>
-        <v>11.4431904523637</v>
+        <v>10.7684164308713</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="n">
-        <v>4.239014</v>
+        <v>5.234588</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>4.314815</v>
+        <v>4.324302</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>4.457629</v>
+        <v>4.362406</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>4.305167</v>
+        <v>4.654169</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>4.682572</v>
+        <v>4.196198</v>
       </c>
       <c r="H34" s="0" t="n">
         <f aca="false">MIN(C34:G34)</f>
-        <v>4.239014</v>
+        <v>4.196198</v>
       </c>
       <c r="I34" s="0" t="n">
         <f aca="false">MAX(C34:G34)</f>
-        <v>4.682572</v>
+        <v>5.234588</v>
       </c>
       <c r="J34" s="0" t="n">
         <f aca="false">AVERAGE(C34:G34)</f>
-        <v>4.3998394</v>
+        <v>4.5543326</v>
       </c>
       <c r="K34" s="0" t="n">
         <f aca="false">J$34/J34</f>
@@ -2034,167 +2547,761 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="n">
-        <v>2.545573</v>
+        <v>3.029614</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>2.25481</v>
+        <v>2.769981</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>2.658885</v>
+        <v>3.105322</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>3.092724</v>
+        <v>3.083377</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>2.744111</v>
+        <v>2.642619</v>
       </c>
       <c r="H35" s="0" t="n">
         <f aca="false">MIN(C35:G35)</f>
-        <v>2.25481</v>
+        <v>2.642619</v>
       </c>
       <c r="I35" s="0" t="n">
         <f aca="false">MAX(C35:G35)</f>
-        <v>3.092724</v>
+        <v>3.105322</v>
       </c>
       <c r="J35" s="0" t="n">
         <f aca="false">AVERAGE(C35:G35)</f>
-        <v>2.6592206</v>
+        <v>2.9261826</v>
       </c>
       <c r="K35" s="0" t="n">
         <f aca="false">J$34/J35</f>
-        <v>1.65455976085625</v>
+        <v>1.55640751879257</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="n">
-        <v>1.421313</v>
+        <v>1.772203</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>1.444731</v>
+        <v>1.321035</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>1.274096</v>
+        <v>1.802325</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>1.717007</v>
+        <v>1.738009</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>1.642137</v>
+        <v>1.864171</v>
       </c>
       <c r="H36" s="0" t="n">
         <f aca="false">MIN(C36:G36)</f>
-        <v>1.274096</v>
+        <v>1.321035</v>
       </c>
       <c r="I36" s="0" t="n">
         <f aca="false">MAX(C36:G36)</f>
-        <v>1.717007</v>
+        <v>1.864171</v>
       </c>
       <c r="J36" s="0" t="n">
         <f aca="false">AVERAGE(C36:G36)</f>
-        <v>1.4998568</v>
+        <v>1.6995486</v>
       </c>
       <c r="K36" s="0" t="n">
         <f aca="false">J$34/J36</f>
-        <v>2.93350631873656</v>
+        <v>2.67973072379336</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="n">
-        <v>0.779178</v>
+        <v>0.877931</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0.80127</v>
+        <v>0.778885</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>0.791778</v>
+        <v>0.918102</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>0.936526</v>
+        <v>0.972468</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>0.937668</v>
+        <v>0.883853</v>
       </c>
       <c r="H37" s="0" t="n">
         <f aca="false">MIN(C37:G37)</f>
-        <v>0.779178</v>
+        <v>0.778885</v>
       </c>
       <c r="I37" s="0" t="n">
         <f aca="false">MAX(C37:G37)</f>
-        <v>0.937668</v>
+        <v>0.972468</v>
       </c>
       <c r="J37" s="0" t="n">
         <f aca="false">AVERAGE(C37:G37)</f>
-        <v>0.849284</v>
+        <v>0.8862478</v>
       </c>
       <c r="K37" s="0" t="n">
         <f aca="false">J$34/J37</f>
-        <v>5.18064557909957</v>
+        <v>5.13889298230134</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="n">
-        <v>0.614002</v>
+        <v>0.699723</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>0.620821</v>
+        <v>0.653243</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>0.617994</v>
+        <v>0.70307</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>0.669183</v>
+        <v>0.697914</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>0.642563</v>
+        <v>0.754102</v>
       </c>
       <c r="H38" s="0" t="n">
         <f aca="false">MIN(C38:G38)</f>
-        <v>0.614002</v>
+        <v>0.653243</v>
       </c>
       <c r="I38" s="0" t="n">
         <f aca="false">MAX(C38:G38)</f>
-        <v>0.669183</v>
+        <v>0.754102</v>
       </c>
       <c r="J38" s="0" t="n">
         <f aca="false">AVERAGE(C38:G38)</f>
-        <v>0.6329126</v>
+        <v>0.7016104</v>
       </c>
       <c r="K38" s="0" t="n">
         <f aca="false">J$34/J38</f>
-        <v>6.95173298809346</v>
+        <v>6.49125583087138</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="n">
-        <v>0.344651</v>
+        <v>0.361998</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0.386732</v>
+        <v>0.371074</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>0.385637</v>
+        <v>0.371004</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>0.393532</v>
+        <v>0.398589</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>0.361472</v>
+        <v>0.369003</v>
       </c>
       <c r="H39" s="0" t="n">
         <f aca="false">MIN(C39:G39)</f>
-        <v>0.344651</v>
+        <v>0.361998</v>
       </c>
       <c r="I39" s="0" t="n">
         <f aca="false">MAX(C39:G39)</f>
-        <v>0.393532</v>
+        <v>0.398589</v>
       </c>
       <c r="J39" s="0" t="n">
         <f aca="false">AVERAGE(C39:G39)</f>
-        <v>0.3744048</v>
+        <v>0.3743336</v>
       </c>
       <c r="K39" s="0" t="n">
         <f aca="false">J$34/J39</f>
-        <v>11.7515571381564</v>
+        <v>12.1665076284897</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="0" t="n">
+        <v>0.29719</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>0.287602</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0.286019</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0.262991</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0.285148</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <f aca="false">MIN(C42:G42)</f>
+        <v>0.262991</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <f aca="false">MAX(C42:G42)</f>
+        <v>0.29719</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <f aca="false">AVERAGE(C42:G42)</f>
+        <v>0.28379</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <f aca="false">J$42/J42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="0" t="n">
+        <v>0.177317</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>0.180798</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>0.175222</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0.173773</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>0.175134</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <f aca="false">MIN(C43:G43)</f>
+        <v>0.173773</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <f aca="false">MAX(C43:G43)</f>
+        <v>0.180798</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <f aca="false">AVERAGE(C43:G43)</f>
+        <v>0.1764488</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <f aca="false">J$42/J43</f>
+        <v>1.60834190994781</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="0" t="n">
+        <v>0.153809</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>0.147095</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>0.145134</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0.155647</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>0.146571</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <f aca="false">MIN(C44:G44)</f>
+        <v>0.145134</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <f aca="false">MAX(C44:G44)</f>
+        <v>0.155647</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <f aca="false">AVERAGE(C44:G44)</f>
+        <v>0.1496512</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <f aca="false">J$42/J44</f>
+        <v>1.89634296283625</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="0" t="n">
+        <v>0.091342</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>0.094596</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>0.089481</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>0.087837</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>0.086603</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <f aca="false">MIN(C45:G45)</f>
+        <v>0.086603</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <f aca="false">MAX(C45:G45)</f>
+        <v>0.094596</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <f aca="false">AVERAGE(C45:G45)</f>
+        <v>0.0899718</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <f aca="false">J$42/J45</f>
+        <v>3.15421054152523</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="0" t="n">
+        <v>0.054971</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>0.053193</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>0.053556</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>0.056011</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>0.054462</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <f aca="false">MIN(C46:G46)</f>
+        <v>0.053193</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <f aca="false">MAX(C46:G46)</f>
+        <v>0.056011</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <f aca="false">AVERAGE(C46:G46)</f>
+        <v>0.0544386</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <f aca="false">J$42/J46</f>
+        <v>5.21302899045898</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="0" t="n">
+        <v>0.04494</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>0.045225</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>0.04222</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>0.044133</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>0.042371</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <f aca="false">MIN(C47:G47)</f>
+        <v>0.04222</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <f aca="false">MAX(C47:G47)</f>
+        <v>0.045225</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <f aca="false">AVERAGE(C47:G47)</f>
+        <v>0.0437778</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <f aca="false">J$42/J47</f>
+        <v>6.48250939974142</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="0" t="n">
+        <v>2.171124</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>2.169361</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>2.106139</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>2.177651</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>1.977039</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <f aca="false">MIN(C48:G48)</f>
+        <v>1.977039</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <f aca="false">MAX(C48:G48)</f>
+        <v>2.177651</v>
+      </c>
+      <c r="J48" s="0" t="n">
+        <f aca="false">AVERAGE(C48:G48)</f>
+        <v>2.1202628</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <f aca="false">J$48/J48</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="0" t="n">
+        <v>1.181477</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>1.222872</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>1.276784</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>1.17829</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>1.197062</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <f aca="false">MIN(C49:G49)</f>
+        <v>1.17829</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <f aca="false">MAX(C49:G49)</f>
+        <v>1.276784</v>
+      </c>
+      <c r="J49" s="0" t="n">
+        <f aca="false">AVERAGE(C49:G49)</f>
+        <v>1.211297</v>
+      </c>
+      <c r="K49" s="0" t="n">
+        <f aca="false">J$48/J49</f>
+        <v>1.75040704302908</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="0" t="n">
+        <v>0.970645</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>1.005038</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>0.985992</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>0.997624</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>0.984814</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <f aca="false">MIN(C50:G50)</f>
+        <v>0.970645</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <f aca="false">MAX(C50:G50)</f>
+        <v>1.005038</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <f aca="false">AVERAGE(C50:G50)</f>
+        <v>0.9888226</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <f aca="false">J$48/J50</f>
+        <v>2.14422971319628</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="0" t="n">
+        <v>0.550597</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>0.546612</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>0.543845</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>0.548572</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>0.546885</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <f aca="false">MIN(C51:G51)</f>
+        <v>0.543845</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <f aca="false">MAX(C51:G51)</f>
+        <v>0.550597</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <f aca="false">AVERAGE(C51:G51)</f>
+        <v>0.5473022</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <f aca="false">J$48/J51</f>
+        <v>3.87402572107329</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="0" t="n">
+        <v>0.292649</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0.299175</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>0.300618</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>0.301418</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>0.302464</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <f aca="false">MIN(C52:G52)</f>
+        <v>0.292649</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <f aca="false">MAX(C52:G52)</f>
+        <v>0.302464</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <f aca="false">AVERAGE(C52:G52)</f>
+        <v>0.2992648</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <f aca="false">J$48/J52</f>
+        <v>7.084905408187</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="0" t="n">
+        <v>0.183647</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0.187215</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>0.198202</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>0.192706</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>0.182903</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <f aca="false">MIN(C53:G53)</f>
+        <v>0.182903</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <f aca="false">MAX(C53:G53)</f>
+        <v>0.198202</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <f aca="false">AVERAGE(C53:G53)</f>
+        <v>0.1889346</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <f aca="false">J$48/J53</f>
+        <v>11.2222049322887</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="0" t="n">
+        <v>4.311294</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>4.330786</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>4.51862</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>4.63625</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>4.313773</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <f aca="false">MIN(C54:G54)</f>
+        <v>4.311294</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <f aca="false">MAX(C54:G54)</f>
+        <v>4.63625</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <f aca="false">AVERAGE(C54:G54)</f>
+        <v>4.4221446</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <f aca="false">J$54/J54</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="0" t="n">
+        <v>3.037922</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>3.076158</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>2.482921</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>2.930647</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>2.726444</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <f aca="false">MIN(C55:G55)</f>
+        <v>2.482921</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <f aca="false">MAX(C55:G55)</f>
+        <v>3.076158</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <f aca="false">AVERAGE(C55:G55)</f>
+        <v>2.8508184</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <f aca="false">J$54/J55</f>
+        <v>1.55118424940712</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="0" t="n">
+        <v>2.231925</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>2.082235</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>2.123572</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>2.148995</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <v>2.081237</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <f aca="false">MIN(C56:G56)</f>
+        <v>2.081237</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <f aca="false">MAX(C56:G56)</f>
+        <v>2.231925</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <f aca="false">AVERAGE(C56:G56)</f>
+        <v>2.1335928</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <f aca="false">J$54/J56</f>
+        <v>2.07262819784544</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="0" t="n">
+        <v>1.128948</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>1.175082</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>1.186489</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>1.223216</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>1.141477</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <f aca="false">MIN(C57:G57)</f>
+        <v>1.128948</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <f aca="false">MAX(C57:G57)</f>
+        <v>1.223216</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <f aca="false">AVERAGE(C57:G57)</f>
+        <v>1.1710424</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <f aca="false">J$54/J57</f>
+        <v>3.77624635965359</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="0" t="n">
+        <v>0.637772</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>0.636536</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>0.633776</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>0.638937</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>0.685732</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <f aca="false">MIN(C58:G58)</f>
+        <v>0.633776</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <f aca="false">MAX(C58:G58)</f>
+        <v>0.685732</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <f aca="false">AVERAGE(C58:G58)</f>
+        <v>0.6465506</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <f aca="false">J$54/J58</f>
+        <v>6.83959553977678</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="0" t="n">
+        <v>0.352444</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>0.36015</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>0.350731</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>0.346828</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>0.362268</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <f aca="false">MIN(C59:G59)</f>
+        <v>0.346828</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <f aca="false">MAX(C59:G59)</f>
+        <v>0.362268</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <f aca="false">AVERAGE(C59:G59)</f>
+        <v>0.3544842</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <f aca="false">J$54/J59</f>
+        <v>12.4748708122957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>